<commit_message>
group data to species and new interface
</commit_message>
<xml_diff>
--- a/pandas_simple.xlsx
+++ b/pandas_simple.xlsx
@@ -1134,7 +1134,7 @@
         <v>80</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>142</v>
@@ -1154,7 +1154,7 @@
         <v>80</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>143</v>
@@ -1174,7 +1174,7 @@
         <v>81</v>
       </c>
       <c r="E4">
-        <v>0.9939613526570048</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="F4" t="s">
         <v>144</v>
@@ -1194,7 +1194,7 @@
         <v>82</v>
       </c>
       <c r="E5">
-        <v>0.9993823347745522</v>
+        <v>99.94</v>
       </c>
       <c r="F5" t="s">
         <v>145</v>
@@ -1214,7 +1214,7 @@
         <v>83</v>
       </c>
       <c r="E6">
-        <v>0.9921497584541062</v>
+        <v>99.20999999999999</v>
       </c>
       <c r="F6" t="s">
         <v>146</v>
@@ -1234,7 +1234,7 @@
         <v>84</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
         <v>147</v>
@@ -1254,7 +1254,7 @@
         <v>85</v>
       </c>
       <c r="E8">
-        <v>0.9993800371977681</v>
+        <v>99.94</v>
       </c>
       <c r="F8" t="s">
         <v>148</v>
@@ -1274,7 +1274,7 @@
         <v>86</v>
       </c>
       <c r="E9">
-        <v>0.9903381642512077</v>
+        <v>99.03</v>
       </c>
       <c r="F9" t="s">
         <v>149</v>
@@ -1294,7 +1294,7 @@
         <v>87</v>
       </c>
       <c r="E10">
-        <v>0.9969001859888407</v>
+        <v>99.69</v>
       </c>
       <c r="F10" t="s">
         <v>150</v>
@@ -1314,7 +1314,7 @@
         <v>88</v>
       </c>
       <c r="E11">
-        <v>0.9885265700483091</v>
+        <v>98.84999999999999</v>
       </c>
       <c r="F11" t="s">
         <v>151</v>
@@ -1334,7 +1334,7 @@
         <v>89</v>
       </c>
       <c r="E12">
-        <v>0.9830917874396136</v>
+        <v>98.31</v>
       </c>
       <c r="F12" t="s">
         <v>152</v>
@@ -1354,7 +1354,7 @@
         <v>90</v>
       </c>
       <c r="E13">
-        <v>0.9806763285024155</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="F13" t="s">
         <v>153</v>
@@ -1374,7 +1374,7 @@
         <v>90</v>
       </c>
       <c r="E14">
-        <v>0.9806763285024155</v>
+        <v>98.06999999999999</v>
       </c>
       <c r="F14" t="s">
         <v>154</v>
@@ -1394,7 +1394,7 @@
         <v>91</v>
       </c>
       <c r="E15">
-        <v>0.9829164124466138</v>
+        <v>98.29000000000001</v>
       </c>
       <c r="F15" t="s">
         <v>155</v>
@@ -1414,7 +1414,7 @@
         <v>91</v>
       </c>
       <c r="E16">
-        <v>0.9829164124466138</v>
+        <v>98.29000000000001</v>
       </c>
       <c r="F16" t="s">
         <v>156</v>
@@ -1434,7 +1434,7 @@
         <v>91</v>
       </c>
       <c r="E17">
-        <v>0.9829164124466138</v>
+        <v>98.29000000000001</v>
       </c>
       <c r="F17" t="s">
         <v>157</v>
@@ -1454,7 +1454,7 @@
         <v>92</v>
       </c>
       <c r="E18">
-        <v>0.9794685990338164</v>
+        <v>97.95</v>
       </c>
       <c r="F18" t="s">
         <v>158</v>
@@ -1474,7 +1474,7 @@
         <v>93</v>
       </c>
       <c r="E19">
-        <v>0.9810281517747858</v>
+        <v>98.09999999999999</v>
       </c>
       <c r="F19" t="s">
         <v>159</v>
@@ -1494,7 +1494,7 @@
         <v>94</v>
       </c>
       <c r="E20">
-        <v>0.9820877084620135</v>
+        <v>98.20999999999999</v>
       </c>
       <c r="F20" t="s">
         <v>160</v>
@@ -1514,7 +1514,7 @@
         <v>95</v>
       </c>
       <c r="E21">
-        <v>0.9942233632862645</v>
+        <v>99.42</v>
       </c>
       <c r="F21" t="s">
         <v>161</v>
@@ -1534,7 +1534,7 @@
         <v>96</v>
       </c>
       <c r="E22">
-        <v>0.9993394980184941</v>
+        <v>99.93000000000001</v>
       </c>
       <c r="F22" t="s">
         <v>162</v>
@@ -1554,7 +1554,7 @@
         <v>97</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F23" t="s">
         <v>163</v>
@@ -1574,7 +1574,7 @@
         <v>97</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
         <v>164</v>
@@ -1594,7 +1594,7 @@
         <v>97</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F25" t="s">
         <v>165</v>
@@ -1614,7 +1614,7 @@
         <v>97</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
         <v>166</v>
@@ -1634,7 +1634,7 @@
         <v>97</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F27" t="s">
         <v>167</v>
@@ -1654,7 +1654,7 @@
         <v>98</v>
       </c>
       <c r="E28">
-        <v>0.9940554821664465</v>
+        <v>99.41</v>
       </c>
       <c r="F28" t="s">
         <v>168</v>
@@ -1674,7 +1674,7 @@
         <v>98</v>
       </c>
       <c r="E29">
-        <v>0.9940554821664465</v>
+        <v>99.41</v>
       </c>
       <c r="F29" t="s">
         <v>169</v>
@@ -1694,7 +1694,7 @@
         <v>98</v>
       </c>
       <c r="E30">
-        <v>0.9940554821664465</v>
+        <v>99.41</v>
       </c>
       <c r="F30" t="s">
         <v>170</v>
@@ -1714,7 +1714,7 @@
         <v>98</v>
       </c>
       <c r="E31">
-        <v>0.9940554821664465</v>
+        <v>99.41</v>
       </c>
       <c r="F31" t="s">
         <v>171</v>
@@ -1734,7 +1734,7 @@
         <v>99</v>
       </c>
       <c r="E32">
-        <v>0.9920739762219286</v>
+        <v>99.20999999999999</v>
       </c>
       <c r="F32" t="s">
         <v>172</v>
@@ -1754,7 +1754,7 @@
         <v>100</v>
       </c>
       <c r="E33">
-        <v>0.9744707347447074</v>
+        <v>97.45</v>
       </c>
       <c r="F33" t="s">
         <v>173</v>
@@ -1774,7 +1774,7 @@
         <v>101</v>
       </c>
       <c r="E34">
-        <v>0.9625603864734299</v>
+        <v>96.26000000000001</v>
       </c>
       <c r="F34" t="s">
         <v>174</v>
@@ -1794,7 +1794,7 @@
         <v>101</v>
       </c>
       <c r="E35">
-        <v>0.9625603864734299</v>
+        <v>96.26000000000001</v>
       </c>
       <c r="F35" t="s">
         <v>175</v>
@@ -1814,7 +1814,7 @@
         <v>101</v>
       </c>
       <c r="E36">
-        <v>0.9625603864734299</v>
+        <v>96.26000000000001</v>
       </c>
       <c r="F36" t="s">
         <v>176</v>
@@ -1834,7 +1834,7 @@
         <v>102</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F37" t="s">
         <v>177</v>
@@ -1854,7 +1854,7 @@
         <v>103</v>
       </c>
       <c r="E38">
-        <v>0.9939759036144579</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="F38" t="s">
         <v>178</v>
@@ -1874,7 +1874,7 @@
         <v>103</v>
       </c>
       <c r="E39">
-        <v>0.9939759036144579</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="F39" t="s">
         <v>179</v>
@@ -1894,7 +1894,7 @@
         <v>104</v>
       </c>
       <c r="E40">
-        <v>0.961352657004831</v>
+        <v>96.14</v>
       </c>
       <c r="F40" t="s">
         <v>180</v>
@@ -1914,7 +1914,7 @@
         <v>104</v>
       </c>
       <c r="E41">
-        <v>0.961352657004831</v>
+        <v>96.14</v>
       </c>
       <c r="F41" t="s">
         <v>181</v>
@@ -1934,7 +1934,7 @@
         <v>104</v>
       </c>
       <c r="E42">
-        <v>0.961352657004831</v>
+        <v>96.14</v>
       </c>
       <c r="F42" t="s">
         <v>182</v>
@@ -1954,7 +1954,7 @@
         <v>105</v>
       </c>
       <c r="E43">
-        <v>0.9607487922705314</v>
+        <v>96.06999999999999</v>
       </c>
       <c r="F43" t="s">
         <v>183</v>
@@ -1974,7 +1974,7 @@
         <v>106</v>
       </c>
       <c r="E44">
-        <v>0.9919678714859438</v>
+        <v>99.2</v>
       </c>
       <c r="F44" t="s">
         <v>184</v>
@@ -1994,7 +1994,7 @@
         <v>107</v>
       </c>
       <c r="E45">
-        <v>0.9595410628019324</v>
+        <v>95.95</v>
       </c>
       <c r="F45" t="s">
         <v>185</v>
@@ -2014,7 +2014,7 @@
         <v>108</v>
       </c>
       <c r="E46">
-        <v>0.9854689564068693</v>
+        <v>98.55</v>
       </c>
       <c r="F46" t="s">
         <v>186</v>
@@ -2034,7 +2034,7 @@
         <v>108</v>
       </c>
       <c r="E47">
-        <v>0.9854689564068693</v>
+        <v>98.55</v>
       </c>
       <c r="F47" t="s">
         <v>187</v>
@@ -2054,7 +2054,7 @@
         <v>109</v>
       </c>
       <c r="E48">
-        <v>0.9589371980676329</v>
+        <v>95.89</v>
       </c>
       <c r="F48" t="s">
         <v>188</v>
@@ -2074,7 +2074,7 @@
         <v>109</v>
       </c>
       <c r="E49">
-        <v>0.9589371980676329</v>
+        <v>95.89</v>
       </c>
       <c r="F49" t="s">
         <v>189</v>
@@ -2094,7 +2094,7 @@
         <v>109</v>
       </c>
       <c r="E50">
-        <v>0.9589371980676329</v>
+        <v>95.89</v>
       </c>
       <c r="F50" t="s">
         <v>190</v>
@@ -2114,7 +2114,7 @@
         <v>110</v>
       </c>
       <c r="E51">
-        <v>0.9583333333333334</v>
+        <v>95.83</v>
       </c>
       <c r="F51" t="s">
         <v>191</v>
@@ -2134,7 +2134,7 @@
         <v>111</v>
       </c>
       <c r="E52">
-        <v>0.9952348536419333</v>
+        <v>99.52</v>
       </c>
       <c r="F52" t="s">
         <v>192</v>
@@ -2154,7 +2154,7 @@
         <v>112</v>
       </c>
       <c r="E53">
-        <v>0.9705144291091593</v>
+        <v>97.05</v>
       </c>
       <c r="F53" t="s">
         <v>193</v>
@@ -2174,7 +2174,7 @@
         <v>113</v>
       </c>
       <c r="E54">
-        <v>0.9577294685990339</v>
+        <v>95.77</v>
       </c>
       <c r="F54" t="s">
         <v>194</v>
@@ -2194,7 +2194,7 @@
         <v>110</v>
       </c>
       <c r="E55">
-        <v>0.9560240963855422</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="F55" t="s">
         <v>195</v>
@@ -2214,7 +2214,7 @@
         <v>114</v>
       </c>
       <c r="E56">
-        <v>0.9571256038647343</v>
+        <v>95.70999999999999</v>
       </c>
       <c r="F56" t="s">
         <v>196</v>
@@ -2234,7 +2234,7 @@
         <v>115</v>
       </c>
       <c r="E57">
-        <v>0.9859437751004017</v>
+        <v>98.59</v>
       </c>
       <c r="F57" t="s">
         <v>197</v>
@@ -2254,7 +2254,7 @@
         <v>115</v>
       </c>
       <c r="E58">
-        <v>0.9859437751004017</v>
+        <v>98.59</v>
       </c>
       <c r="F58" t="s">
         <v>198</v>
@@ -2274,7 +2274,7 @@
         <v>116</v>
       </c>
       <c r="E59">
-        <v>0.9547101449275363</v>
+        <v>95.47</v>
       </c>
       <c r="F59" t="s">
         <v>199</v>
@@ -2294,7 +2294,7 @@
         <v>116</v>
       </c>
       <c r="E60">
-        <v>0.9547101449275363</v>
+        <v>95.47</v>
       </c>
       <c r="F60" t="s">
         <v>200</v>
@@ -2314,7 +2314,7 @@
         <v>117</v>
       </c>
       <c r="E61">
-        <v>0.9839357429718876</v>
+        <v>98.39</v>
       </c>
       <c r="F61" t="s">
         <v>201</v>
@@ -2334,7 +2334,7 @@
         <v>117</v>
       </c>
       <c r="E62">
-        <v>0.9839357429718876</v>
+        <v>98.39</v>
       </c>
       <c r="F62" t="s">
         <v>202</v>
@@ -2354,7 +2354,7 @@
         <v>118</v>
       </c>
       <c r="E63">
-        <v>0.9565483476132191</v>
+        <v>95.65000000000001</v>
       </c>
       <c r="F63" t="s">
         <v>203</v>
@@ -2374,7 +2374,7 @@
         <v>118</v>
       </c>
       <c r="E64">
-        <v>0.9565483476132191</v>
+        <v>95.65000000000001</v>
       </c>
       <c r="F64" t="s">
         <v>204</v>
@@ -2394,7 +2394,7 @@
         <v>119</v>
       </c>
       <c r="E65">
-        <v>0.9819277108433735</v>
+        <v>98.19</v>
       </c>
       <c r="F65" t="s">
         <v>205</v>
@@ -2414,7 +2414,7 @@
         <v>120</v>
       </c>
       <c r="E66">
-        <v>0.9812583668005355</v>
+        <v>98.13</v>
       </c>
       <c r="F66" t="s">
         <v>206</v>
@@ -2434,7 +2434,7 @@
         <v>121</v>
       </c>
       <c r="E67">
-        <v>0.9547123623011016</v>
+        <v>95.47</v>
       </c>
       <c r="F67" t="s">
         <v>207</v>
@@ -2454,7 +2454,7 @@
         <v>122</v>
       </c>
       <c r="E68">
-        <v>0.9805890227576974</v>
+        <v>98.06</v>
       </c>
       <c r="F68" t="s">
         <v>208</v>
@@ -2474,7 +2474,7 @@
         <v>123</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F69" t="s">
         <v>209</v>
@@ -2494,7 +2494,7 @@
         <v>123</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F70" t="s">
         <v>210</v>
@@ -2514,7 +2514,7 @@
         <v>124</v>
       </c>
       <c r="E71">
-        <v>0.964993394980185</v>
+        <v>96.5</v>
       </c>
       <c r="F71" t="s">
         <v>211</v>
@@ -2534,7 +2534,7 @@
         <v>125</v>
       </c>
       <c r="E72">
-        <v>0.9649702577660277</v>
+        <v>96.5</v>
       </c>
       <c r="F72" t="s">
         <v>212</v>
@@ -2554,7 +2554,7 @@
         <v>126</v>
       </c>
       <c r="E73">
-        <v>0.9844961240310077</v>
+        <v>98.45</v>
       </c>
       <c r="F73" t="s">
         <v>213</v>
@@ -2574,7 +2574,7 @@
         <v>127</v>
       </c>
       <c r="E74">
-        <v>0.9851590106007068</v>
+        <v>98.52</v>
       </c>
       <c r="F74" t="s">
         <v>214</v>
@@ -2594,7 +2594,7 @@
         <v>128</v>
       </c>
       <c r="E75">
-        <v>0.9636723910171731</v>
+        <v>96.37</v>
       </c>
       <c r="F75" t="s">
         <v>215</v>
@@ -2614,7 +2614,7 @@
         <v>129</v>
       </c>
       <c r="E76">
-        <v>0.9636483807005949</v>
+        <v>96.36</v>
       </c>
       <c r="F76" t="s">
         <v>216</v>
@@ -2634,7 +2634,7 @@
         <v>130</v>
       </c>
       <c r="E77">
-        <v>0.9616908850726552</v>
+        <v>96.17</v>
       </c>
       <c r="F77" t="s">
         <v>217</v>
@@ -2654,7 +2654,7 @@
         <v>130</v>
       </c>
       <c r="E78">
-        <v>0.9616908850726552</v>
+        <v>96.17</v>
       </c>
       <c r="F78" t="s">
         <v>218</v>
@@ -2674,7 +2674,7 @@
         <v>130</v>
       </c>
       <c r="E79">
-        <v>0.9616908850726552</v>
+        <v>96.17</v>
       </c>
       <c r="F79" t="s">
         <v>219</v>
@@ -2694,7 +2694,7 @@
         <v>130</v>
       </c>
       <c r="E80">
-        <v>0.9616908850726552</v>
+        <v>96.17</v>
       </c>
       <c r="F80" t="s">
         <v>220</v>
@@ -2714,7 +2714,7 @@
         <v>131</v>
       </c>
       <c r="E81">
-        <v>0.9616655651024455</v>
+        <v>96.17</v>
       </c>
       <c r="F81" t="s">
         <v>221</v>
@@ -2734,7 +2734,7 @@
         <v>132</v>
       </c>
       <c r="E82">
-        <v>0.964524765729585</v>
+        <v>96.45</v>
       </c>
       <c r="F82" t="s">
         <v>222</v>
@@ -2754,7 +2754,7 @@
         <v>132</v>
       </c>
       <c r="E83">
-        <v>0.964524765729585</v>
+        <v>96.45</v>
       </c>
       <c r="F83" t="s">
         <v>223</v>
@@ -2774,7 +2774,7 @@
         <v>132</v>
       </c>
       <c r="E84">
-        <v>0.964524765729585</v>
+        <v>96.45</v>
       </c>
       <c r="F84" t="s">
         <v>224</v>
@@ -2794,7 +2794,7 @@
         <v>132</v>
       </c>
       <c r="E85">
-        <v>0.964524765729585</v>
+        <v>96.45</v>
       </c>
       <c r="F85" t="s">
         <v>225</v>
@@ -2814,7 +2814,7 @@
         <v>133</v>
       </c>
       <c r="E86">
-        <v>0.963855421686747</v>
+        <v>96.39</v>
       </c>
       <c r="F86" t="s">
         <v>226</v>
@@ -2834,7 +2834,7 @@
         <v>134</v>
       </c>
       <c r="E87">
-        <v>0.9597093791281374</v>
+        <v>95.97</v>
       </c>
       <c r="F87" t="s">
         <v>227</v>
@@ -2854,7 +2854,7 @@
         <v>135</v>
       </c>
       <c r="E88">
-        <v>0.9613590939373751</v>
+        <v>96.14</v>
       </c>
       <c r="F88" t="s">
         <v>228</v>
@@ -2874,7 +2874,7 @@
         <v>136</v>
       </c>
       <c r="E89">
-        <v>0.963186077643909</v>
+        <v>96.31999999999999</v>
       </c>
       <c r="F89" t="s">
         <v>229</v>
@@ -2894,7 +2894,7 @@
         <v>136</v>
       </c>
       <c r="E90">
-        <v>0.9625418060200669</v>
+        <v>96.25</v>
       </c>
       <c r="F90" t="s">
         <v>230</v>
@@ -2914,7 +2914,7 @@
         <v>137</v>
       </c>
       <c r="E91">
-        <v>0.9605878423513694</v>
+        <v>96.06</v>
       </c>
       <c r="F91" t="s">
         <v>231</v>
@@ -2934,7 +2934,7 @@
         <v>112</v>
       </c>
       <c r="E92">
-        <v>0.9280143971205759</v>
+        <v>92.8</v>
       </c>
       <c r="F92" t="s">
         <v>232</v>
@@ -2954,7 +2954,7 @@
         <v>112</v>
       </c>
       <c r="E93">
-        <v>0.9280143971205759</v>
+        <v>92.8</v>
       </c>
       <c r="F93" t="s">
         <v>233</v>
@@ -2974,7 +2974,7 @@
         <v>138</v>
       </c>
       <c r="E94">
-        <v>0.9845588235294118</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="F94" t="s">
         <v>234</v>
@@ -2994,7 +2994,7 @@
         <v>138</v>
       </c>
       <c r="E95">
-        <v>0.9845588235294118</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="F95" t="s">
         <v>235</v>
@@ -3014,7 +3014,7 @@
         <v>139</v>
       </c>
       <c r="E96">
-        <v>0.9838235294117647</v>
+        <v>98.38</v>
       </c>
       <c r="F96" t="s">
         <v>236</v>
@@ -3034,7 +3034,7 @@
         <v>140</v>
       </c>
       <c r="E97">
-        <v>0.9262147570485902</v>
+        <v>92.62</v>
       </c>
       <c r="F97" t="s">
         <v>237</v>
@@ -3054,7 +3054,7 @@
         <v>140</v>
       </c>
       <c r="E98">
-        <v>0.9262147570485902</v>
+        <v>92.62</v>
       </c>
       <c r="F98" t="s">
         <v>238</v>
@@ -3074,7 +3074,7 @@
         <v>140</v>
       </c>
       <c r="E99">
-        <v>0.9262147570485902</v>
+        <v>92.62</v>
       </c>
       <c r="F99" t="s">
         <v>239</v>
@@ -3094,7 +3094,7 @@
         <v>140</v>
       </c>
       <c r="E100">
-        <v>0.9262147570485902</v>
+        <v>92.62</v>
       </c>
       <c r="F100" t="s">
         <v>240</v>
@@ -3114,7 +3114,7 @@
         <v>141</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F101" t="s">
         <v>241</v>

</xml_diff>